<commit_message>
Modified code for non UK delivery
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{634FA587-4B62-4B1A-8685-F48194BE0225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EFE00CDF-B4DE-4381-85F6-25CC210A4A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
   </bookViews>
   <sheets>
     <sheet name="placeOrder" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>searchKey</t>
   </si>
@@ -59,9 +59,6 @@
     <t>hp</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>United Kingdom</t>
   </si>
   <si>
@@ -71,13 +68,10 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>mac</t>
-  </si>
-  <si>
-    <t>MacBook Pro</t>
-  </si>
-  <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -113,12 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,21 +424,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92351CC5-02AD-4DED-B1F4-C270FFB57622}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,13 +449,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -474,62 +465,79 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding test for multiple items
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -3,15 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{EFE00CDF-B4DE-4381-85F6-25CC210A4A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\eclipse-workspace\opencartFramework\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A80125-F7DC-4365-9055-E1DD07E54091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
   </bookViews>
   <sheets>
     <sheet name="placeOrder" sheetId="1" r:id="rId1"/>
+    <sheet name="placeMultipleItems" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>searchKey</t>
   </si>
@@ -69,9 +74,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
 </sst>
 </file>
@@ -424,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92351CC5-02AD-4DED-B1F4-C270FFB57622}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,19 +459,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -482,62 +484,94 @@
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AF882C-5F39-4481-8826-AAC46A72753D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added end to end test for guest user
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\eclipse-workspace\opencartFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A80125-F7DC-4365-9055-E1DD07E54091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A76A867-E2D4-41AB-BC2A-6DE9245C3E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
   </bookViews>
   <sheets>
     <sheet name="placeOrder" sheetId="1" r:id="rId1"/>
-    <sheet name="placeMultipleItems" sheetId="2" r:id="rId2"/>
+    <sheet name="placeOrderGuest" sheetId="4" r:id="rId2"/>
+    <sheet name="placeMultipleItems" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>searchKey</t>
   </si>
@@ -74,6 +75,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>BillingAndDeliveryAddressSame</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -429,18 +439,18 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -474,7 +484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -491,7 +501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -514,23 +524,85 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EF170D-3A33-4165-AB33-CE11C664AD28}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AF882C-5F39-4481-8826-AAC46A72753D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -552,7 +624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -563,7 +635,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Added Tests for Guest User Placing Order
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testData.xlsx
+++ b/src/test/resources/testdata/testData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\eclipse-workspace\opencartFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A76A867-E2D4-41AB-BC2A-6DE9245C3E82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE808F4-CC5F-470D-AD28-1B111467B254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{17941467-072C-4973-BFAB-1F372AE0FB34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="placeOrder" sheetId="1" r:id="rId1"/>
-    <sheet name="placeOrderGuest" sheetId="4" r:id="rId2"/>
-    <sheet name="placeMultipleItems" sheetId="2" r:id="rId3"/>
+    <sheet name="placeMultipleItems" sheetId="1" r:id="rId1"/>
+    <sheet name="placeOrder" sheetId="2" r:id="rId2"/>
+    <sheet name="placeOrderGuest" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>searchKey</t>
   </si>
@@ -38,43 +38,34 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>sony</t>
+  </si>
+  <si>
+    <t>Sony VAIO</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>HP LP3065</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Billing Country</t>
+  </si>
+  <si>
     <t>Delivery Country</t>
   </si>
   <si>
-    <t>sony</t>
-  </si>
-  <si>
-    <t>Sony VAIO</t>
-  </si>
-  <si>
-    <t>ipod</t>
-  </si>
-  <si>
-    <t>iPod Classic</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>HP LP3065</t>
-  </si>
-  <si>
-    <t>hp</t>
-  </si>
-  <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>Billing Country</t>
-  </si>
-  <si>
     <t>Japan</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
   <si>
     <t>BillingAndDeliveryAddressSame</t>
@@ -156,7 +147,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -168,7 +159,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -215,23 +206,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -267,23 +241,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,11 +392,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92351CC5-02AD-4DED-B1F4-C270FFB57622}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D854C87B-4712-406A-80D2-17ED42CA6742}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,24 +471,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -486,10 +496,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -498,24 +508,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -523,13 +516,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EF170D-3A33-4165-AB33-CE11C664AD28}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A0DACC-3698-49A8-B40E-DB7E5CE67C03}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -549,101 +540,35 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AF882C-5F39-4481-8826-AAC46A72753D}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>